<commit_message>
Added all test stubs and some tests
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaely\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaely\Downloads\Fall 2023\CSCI 306 SE\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97E0B595-1F28-48A4-8FE7-9410135C2F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B7467-2BA0-4531-94BD-7982118AC211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="44">
   <si>
     <t>W</t>
   </si>
@@ -147,6 +147,27 @@
   </si>
   <si>
     <t>KC</t>
+  </si>
+  <si>
+    <t>Number of Doors: 16</t>
+  </si>
+  <si>
+    <t>White: door direction tests (in FileInitTests)</t>
+  </si>
+  <si>
+    <t>Yellow: room test (in FileInitTests)</t>
+  </si>
+  <si>
+    <t>Light Purple: adjacency from rooms and doors</t>
+  </si>
+  <si>
+    <t>Dark Purple: adjacency from walkways</t>
+  </si>
+  <si>
+    <t>Light Blue: targets from rooms and doors</t>
+  </si>
+  <si>
+    <t>Pink: targets with occupied</t>
   </si>
 </sst>
 </file>
@@ -162,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -205,6 +226,48 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFAFE7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7C35B1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -218,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -226,12 +289,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+      <color rgb="FF7C35B1"/>
+      <color rgb="FFCFAFE7"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -540,18 +617,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="25" width="6.77734375" customWidth="1"/>
+    <col min="27" max="27" width="43.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -624,8 +702,11 @@
       <c r="Y1">
         <v>23</v>
       </c>
+      <c r="AA1" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -644,7 +725,7 @@
       <c r="F2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="3" t="s">
@@ -662,7 +743,7 @@
       <c r="L2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>25</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -701,15 +782,18 @@
       <c r="Y2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="AA2" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -778,8 +862,11 @@
       <c r="Y3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="AA3" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -792,7 +879,7 @@
       <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="7" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -807,7 +894,7 @@
       <c r="I4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="12" t="s">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
@@ -828,7 +915,7 @@
       <c r="P4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="R4" s="2" t="s">
@@ -843,7 +930,7 @@
       <c r="U4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="V4" s="5" t="s">
+      <c r="V4" s="7" t="s">
         <v>29</v>
       </c>
       <c r="W4" s="2" t="s">
@@ -856,7 +943,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -872,7 +959,7 @@
       <c r="E5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="9" t="s">
         <v>17</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -932,8 +1019,11 @@
       <c r="Y5" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="AA5" s="9" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1009,8 +1099,11 @@
       <c r="Y6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="AA6" s="11" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="7" spans="1:25" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1026,7 +1119,7 @@
       <c r="E7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -1077,17 +1170,20 @@
       <c r="V7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W7" s="4" t="s">
+      <c r="W7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="X7" s="3" t="s">
-        <v>0</v>
+      <c r="X7" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="AA7" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1154,17 +1250,20 @@
       <c r="V8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="W8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X8" s="3" t="s">
-        <v>0</v>
+      <c r="W8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="Y8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="AA8" s="13" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1241,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1290,7 +1389,7 @@
       <c r="P10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="Q10" s="13" t="s">
         <v>0</v>
       </c>
       <c r="R10" s="2" t="s">
@@ -1318,7 +1417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1346,7 +1445,7 @@
       <c r="I11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="K11" s="1" t="s">
@@ -1395,7 +1494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1429,7 +1528,7 @@
       <c r="K12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="7" t="s">
         <v>6</v>
       </c>
       <c r="M12" s="1" t="s">
@@ -1441,10 +1540,10 @@
       <c r="O12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="4" t="s">
+      <c r="P12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="12" t="s">
         <v>14</v>
       </c>
       <c r="R12" s="2" t="s">
@@ -1459,7 +1558,7 @@
       <c r="U12" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="V12" s="5" t="s">
+      <c r="V12" s="12" t="s">
         <v>26</v>
       </c>
       <c r="W12" s="2" t="s">
@@ -1472,7 +1571,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1521,7 +1620,7 @@
       <c r="P13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="Q13" s="3" t="s">
+      <c r="Q13" s="13" t="s">
         <v>0</v>
       </c>
       <c r="R13" s="2" t="s">
@@ -1549,7 +1648,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1626,7 +1725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1703,7 +1802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1773,7 +1872,7 @@
       <c r="W16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="X16" s="4" t="s">
+      <c r="X16" s="13" t="s">
         <v>4</v>
       </c>
       <c r="Y16" s="3" t="s">
@@ -1790,7 +1889,7 @@
       <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D17" s="11" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
@@ -1879,7 +1978,7 @@
       <c r="G18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="8" t="s">
         <v>7</v>
       </c>
       <c r="I18" s="3" t="s">
@@ -1903,7 +2002,7 @@
       <c r="O18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="P18" s="3" t="s">
+      <c r="P18" s="12" t="s">
         <v>0</v>
       </c>
       <c r="Q18" s="3" t="s">
@@ -2172,7 +2271,7 @@
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -2187,13 +2286,13 @@
       <c r="G22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="H22" s="12" t="s">
         <v>22</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K22" s="2" t="s">
@@ -2202,7 +2301,7 @@
       <c r="L22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M22" s="5" t="s">
+      <c r="M22" s="9" t="s">
         <v>13</v>
       </c>
       <c r="N22" s="2" t="s">
@@ -2270,7 +2369,7 @@
       <c r="I23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K23" s="2" t="s">
@@ -2347,7 +2446,7 @@
       <c r="I24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="11" t="s">
         <v>0</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -2409,7 +2508,7 @@
       <c r="D25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="11" t="s">
         <v>0</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -2475,5 +2574,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>